<commit_message>
finished 2020 mammal Y/N
</commit_message>
<xml_diff>
--- a/Species Names.xlsx
+++ b/Species Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelly\Documents\Duke\Master's Project\Belize-MP-Bruno-Boos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F381A422-6517-48B7-991D-8F18B01F0B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502AADF6-C229-4DA7-B13A-135FDEACE403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
   <si>
     <t>Type</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Green Heron</t>
+  </si>
+  <si>
+    <t>Brown-headed Flycatcher</t>
   </si>
 </sst>
 </file>
@@ -706,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -810,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -818,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -826,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -834,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -842,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -850,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -858,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -866,23 +869,23 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -890,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -898,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -906,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -914,10 +917,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -925,10 +925,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -936,10 +936,10 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -955,7 +955,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -963,10 +966,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -974,10 +974,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -985,7 +982,10 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -993,7 +993,10 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1001,7 +1004,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1009,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1017,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1025,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1033,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1041,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1049,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1057,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1065,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1073,7 +1076,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1081,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1089,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1097,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1105,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1113,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1121,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1129,7 +1132,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1137,7 +1140,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1145,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1153,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1161,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1169,10 +1172,7 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1180,7 +1180,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1188,7 +1188,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1196,23 +1199,23 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1220,7 +1223,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1228,7 +1231,7 @@
         <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1236,10 +1239,7 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1247,7 +1247,7 @@
         <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,10 @@
         <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>8</v>
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1263,7 +1266,7 @@
         <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1271,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1279,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1287,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -1295,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1303,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1311,7 +1314,7 @@
         <v>5</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -1319,7 +1322,7 @@
         <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1327,7 +1330,7 @@
         <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1335,7 +1338,7 @@
         <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -1343,7 +1346,7 @@
         <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -1351,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -1359,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -1367,10 +1370,7 @@
         <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
-      </c>
-      <c r="C78" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1378,7 +1378,10 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C79" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1386,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -1394,7 +1397,7 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -1402,7 +1405,7 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1410,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1418,7 +1421,7 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1426,7 +1429,7 @@
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -1434,7 +1437,7 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1442,7 +1445,7 @@
         <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -1450,7 +1453,7 @@
         <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -1458,7 +1461,7 @@
         <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -1466,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -1474,7 +1477,7 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -1482,7 +1485,7 @@
         <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -1490,10 +1493,7 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
-      </c>
-      <c r="C93" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -1501,7 +1501,10 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>102</v>
+      </c>
+      <c r="C94" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -1509,7 +1512,7 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -1517,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -1525,15 +1528,15 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -1541,16 +1544,24 @@
         <v>31</v>
       </c>
       <c r="B99" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" t="s">
         <v>32</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C99">
-    <sortCondition ref="A2:A99"/>
-    <sortCondition ref="B2:B99"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C100">
+    <sortCondition ref="A2:A100"/>
+    <sortCondition ref="B2:B100"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>